<commit_message>
recent changes - prior to the presentation and BFS-like configuration generation
</commit_message>
<xml_diff>
--- a/SensorsSchedulerOutLight.xlsx
+++ b/SensorsSchedulerOutLight.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="9780" tabRatio="761" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="9780" tabRatio="761" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralData" sheetId="4" r:id="rId1"/>
@@ -6377,10 +6377,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E22"/>
+      <selection activeCell="A3" sqref="A3:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6421,41 +6421,41 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
       <c r="E3">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>5.0000625000000003</v>
+        <v>9.75</v>
       </c>
       <c r="E4">
-        <v>6.0000625000000003</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6464,259 +6464,259 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>6.0000625000000003</v>
+        <v>10.75</v>
       </c>
       <c r="E5">
-        <v>8.5</v>
+        <v>11.006944444444445</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
       <c r="D6">
-        <v>8.5</v>
+        <v>11.006944444444445</v>
       </c>
       <c r="E6">
-        <v>10.25</v>
+        <v>19.006944444444443</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>10.250152777777778</v>
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>11.250152777777778</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>11.250152777777778</v>
+        <v>15</v>
       </c>
       <c r="E8">
-        <v>12.750152777777778</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>12.750298611111111</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>13.750298611111111</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>18.5</v>
       </c>
       <c r="E10">
-        <v>14</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>18.25</v>
       </c>
       <c r="E11">
-        <v>14.25</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>14.25</v>
+        <v>19.25</v>
       </c>
       <c r="E12">
-        <v>15.75</v>
+        <v>19.354166666666668</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
         <v>3</v>
       </c>
-      <c r="B13">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
       <c r="D13">
-        <v>10.5</v>
+        <v>19.354166666666668</v>
       </c>
       <c r="E13">
-        <v>11.75</v>
+        <v>20.354166666666668</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>11.75</v>
+        <v>12.645833333333334</v>
       </c>
       <c r="E14">
-        <v>12</v>
+        <v>13.645833333333334</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>12</v>
       </c>
       <c r="E15">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E16">
-        <v>18</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>18</v>
+        <v>16.5</v>
       </c>
       <c r="E17">
-        <v>19</v>
+        <v>16.604166666666668</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B18">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18">
-        <v>19.000104166666667</v>
+        <v>16.604166666666668</v>
       </c>
       <c r="E18">
-        <v>20.250104166666667</v>
+        <v>17.604166666666668</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>12</v>
+        <v>17.604166666666668</v>
       </c>
       <c r="E19">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>18</v>
@@ -6727,35 +6727,154 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>19.000076388888889</v>
+        <v>19</v>
       </c>
       <c r="E21">
-        <v>20.500076388888889</v>
+        <v>19.076388888888889</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>19.076388888888889</v>
+      </c>
+      <c r="E22">
+        <v>20.576388888888889</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>18.25</v>
+      </c>
+      <c r="E23">
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>19.25</v>
+      </c>
+      <c r="E24">
+        <v>19.604166666666668</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>19.604166666666668</v>
+      </c>
+      <c r="E25">
+        <v>20.604166666666668</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26">
         <v>6</v>
       </c>
-      <c r="B22">
+      <c r="D26">
+        <v>15</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>18</v>
+      </c>
+      <c r="E28">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
         <v>11</v>
       </c>
-      <c r="C22">
+      <c r="C29">
         <v>3</v>
       </c>
-      <c r="D22">
+      <c r="D29">
         <v>19</v>
       </c>
-      <c r="E22">
+      <c r="E29">
         <v>20</v>
       </c>
     </row>

</xml_diff>